<commit_message>
Try to compile challenge
</commit_message>
<xml_diff>
--- a/robot_c/power_test.xlsx
+++ b/robot_c/power_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\markd\Documents\GitHub\ArticusMaximus\robot_c\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7B9E2638-DA02-4FCE-99CB-538FE10B8AAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF62956A-249C-4589-BB1F-5F5400F688B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{DA3221DA-B51C-41C5-BD7C-382394CC7EC8}"/>
   </bookViews>
@@ -3520,8 +3520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1D13337-3794-4CB1-8C36-E25BF485DA24}">
   <dimension ref="B3:S104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="77" workbookViewId="0">
-      <selection activeCell="Z39" sqref="Z39"/>
+    <sheetView tabSelected="1" zoomScale="59" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>